<commit_message>
Lập lịch gửi dashboard
</commit_message>
<xml_diff>
--- a/Services/Server/Server.API/wwwroot/Reports/BAOCAOTONGQUAN.xlsx
+++ b/Services/Server/Server.API/wwwroot/Reports/BAOCAOTONGQUAN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ACS Solutions\Projects\AMMS_DiemDanhHocSinh\Services\Server\Server.API\wwwroot\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA03C00B-97CA-4B57-8781-253783BBED75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C58C91-729E-4499-A1C0-DDC1E5645CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,16 +27,143 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
+    <t>BÁO CÁO TỔNG QUAN</t>
+  </si>
+  <si>
+    <t>Dữ liệu</t>
+  </si>
+  <si>
+    <t>Trường học</t>
+  </si>
+  <si>
+    <t>Tổng số trường</t>
+  </si>
+  <si>
+    <t>Tổng số lớp</t>
+  </si>
+  <si>
+    <t>Tổng số học sinh</t>
+  </si>
+  <si>
+    <t>{{item.TotalSchoolModel.TotalClass}}</t>
+  </si>
+  <si>
+    <t>Thiết bị</t>
+  </si>
+  <si>
+    <t>Tổng số thiết bị</t>
+  </si>
+  <si>
+    <t>Số thiết bị ZKTeco</t>
+  </si>
+  <si>
+    <t>Số thiết bị Hanet</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>Số thiết bị</t>
+  </si>
+  <si>
+    <t>Offline</t>
+  </si>
+  <si>
+    <t>{{item.DBDeviceModel1.TotalDevice}}</t>
+  </si>
+  <si>
+    <t>{{item.DBDeviceModel1.TotalHN}}</t>
+  </si>
+  <si>
+    <t>{{item.DBDeviceModel1.TotalHNOn}}</t>
+  </si>
+  <si>
+    <t>{{item.DBDeviceModel1.TotalHNOff}}</t>
+  </si>
+  <si>
+    <t>{{item.DBDeviceModel1.TotalZK}}</t>
+  </si>
+  <si>
+    <t>{{item.DBDeviceModel1.TotalZKOn}}</t>
+  </si>
+  <si>
+    <t>{{item.DBDeviceModel1.TotalZKOff}}</t>
+  </si>
+  <si>
+    <t>Hoạt động</t>
+  </si>
+  <si>
+    <t>Đồng bộ khuôn mặt</t>
+  </si>
+  <si>
+    <t>Đã có khuôn mặt</t>
+  </si>
+  <si>
+    <t>Chưa có khuôn mặt</t>
+  </si>
+  <si>
+    <t>{{item.DBStudentFaceModel.TotalStudent}}</t>
+  </si>
+  <si>
+    <t>{{item.DBStudentFaceModel.TotalHasFace}}</t>
+  </si>
+  <si>
+    <t>{{item.DBStudentFaceModel.TotalHasNoFace}}</t>
+  </si>
+  <si>
+    <t>Điểm danh</t>
+  </si>
+  <si>
+    <t>Tổng số học sinh điểm danh</t>
+  </si>
+  <si>
+    <t>Đã đồng bộ</t>
+  </si>
+  <si>
+    <t>Chưa đồng bộ</t>
+  </si>
+  <si>
+    <t>{{item.StudentAttendaceModel.totalAmount}}</t>
+  </si>
+  <si>
+    <t>{{item.StudentAttendaceModel.totalFace}}</t>
+  </si>
+  <si>
+    <t>{{item.StudentAttendaceModel.totalCurrent}}</t>
+  </si>
+  <si>
+    <t>Hệ thống</t>
+  </si>
+  <si>
+    <t>Thống kê gửi email</t>
+  </si>
+  <si>
+    <t>Tổng email đã gửi</t>
+  </si>
+  <si>
+    <t>Số lượng thành công</t>
+  </si>
+  <si>
+    <t>Số lượng thất bại</t>
+  </si>
+  <si>
+    <t>{{item.TotalSendEmailModel.TotalSendEmail}}</t>
+  </si>
+  <si>
+    <t>{{item.TotalSendEmailModel.TotalSendSuccess}}</t>
+  </si>
+  <si>
+    <t>{{item.TotalSendEmailModel.TotalSendFail}}</t>
+  </si>
+  <si>
     <r>
       <rPr>
-        <b/>
         <sz val="12"/>
-        <color indexed="8"/>
+        <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="163"/>
       </rPr>
-      <t xml:space="preserve">Date of report: </t>
+      <t>Time:</t>
     </r>
     <r>
       <rPr>
@@ -44,14 +171,19 @@
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="163"/>
       </rPr>
-      <t>{{date_report}}</t>
+      <t xml:space="preserve">  {{time_report}}</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Time:  </t>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Date of report:</t>
     </r>
     <r>
       <rPr>
@@ -59,145 +191,15 @@
         <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
-        <charset val="163"/>
       </rPr>
-      <t>{{time_report}}</t>
+      <t xml:space="preserve"> {{date_report}}</t>
     </r>
   </si>
   <si>
-    <t>BÁO CÁO TỔNG QUAN</t>
-  </si>
-  <si>
-    <t>Dữ liệu</t>
-  </si>
-  <si>
-    <t>Trường học</t>
-  </si>
-  <si>
-    <t>Tổng số trường</t>
-  </si>
-  <si>
-    <t>Tổng số lớp</t>
-  </si>
-  <si>
-    <t>Tổng số học sinh</t>
-  </si>
-  <si>
     <t>{{item.TotalSchoolModel.TotalSchool}}</t>
   </si>
   <si>
-    <t>{{item.TotalSchoolModel.TotalClass}}</t>
-  </si>
-  <si>
-    <t>{{item.TotalSchoolModel.Student}}</t>
-  </si>
-  <si>
-    <t>Thiết bị</t>
-  </si>
-  <si>
-    <t>Tổng số thiết bị</t>
-  </si>
-  <si>
-    <t>Số thiết bị ZKTeco</t>
-  </si>
-  <si>
-    <t>Số thiết bị Hanet</t>
-  </si>
-  <si>
-    <t>Online</t>
-  </si>
-  <si>
-    <t>Số thiết bị</t>
-  </si>
-  <si>
-    <t>Offline</t>
-  </si>
-  <si>
-    <t>{{item.DBDeviceModel1.TotalDevice}}</t>
-  </si>
-  <si>
-    <t>{{item.DBDeviceModel1.TotalHN}}</t>
-  </si>
-  <si>
-    <t>{{item.DBDeviceModel1.TotalHNOn}}</t>
-  </si>
-  <si>
-    <t>{{item.DBDeviceModel1.TotalHNOff}}</t>
-  </si>
-  <si>
-    <t>{{item.DBDeviceModel1.TotalZK}}</t>
-  </si>
-  <si>
-    <t>{{item.DBDeviceModel1.TotalZKOn}}</t>
-  </si>
-  <si>
-    <t>{{item.DBDeviceModel1.TotalZKOff}}</t>
-  </si>
-  <si>
-    <t>Hoạt động</t>
-  </si>
-  <si>
-    <t>Đồng bộ khuôn mặt</t>
-  </si>
-  <si>
-    <t>Đã có khuôn mặt</t>
-  </si>
-  <si>
-    <t>Chưa có khuôn mặt</t>
-  </si>
-  <si>
-    <t>{{item.DBStudentFaceModel.TotalStudent}}</t>
-  </si>
-  <si>
-    <t>{{item.DBStudentFaceModel.TotalHasFace}}</t>
-  </si>
-  <si>
-    <t>{{item.DBStudentFaceModel.TotalHasNoFace}}</t>
-  </si>
-  <si>
-    <t>Điểm danh</t>
-  </si>
-  <si>
-    <t>Tổng số học sinh điểm danh</t>
-  </si>
-  <si>
-    <t>Đã đồng bộ</t>
-  </si>
-  <si>
-    <t>Chưa đồng bộ</t>
-  </si>
-  <si>
-    <t>{{item.StudentAttendaceModel.totalAmount}}</t>
-  </si>
-  <si>
-    <t>{{item.StudentAttendaceModel.totalFace}}</t>
-  </si>
-  <si>
-    <t>{{item.StudentAttendaceModel.totalCurrent}}</t>
-  </si>
-  <si>
-    <t>Hệ thống</t>
-  </si>
-  <si>
-    <t>Thống kê gửi email</t>
-  </si>
-  <si>
-    <t>Tổng email đã gửi</t>
-  </si>
-  <si>
-    <t>Số lượng thành công</t>
-  </si>
-  <si>
-    <t>Số lượng thất bại</t>
-  </si>
-  <si>
-    <t>{{item.TotalSendEmailModel.TotalSendEmail}}</t>
-  </si>
-  <si>
-    <t>{{item.TotalSendEmailModel.TotalSendSuccess}}</t>
-  </si>
-  <si>
-    <t>{{item.TotalSendEmailModel.TotalSendFail}}</t>
+    <t>{{item.TotalSchoolModel.TotalStudent}}</t>
   </si>
 </sst>
 </file>
@@ -205,9 +207,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="13"/>
       <color indexed="8"/>
@@ -256,16 +258,53 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -288,11 +327,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -304,21 +369,41 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,7 +701,7 @@
   <dimension ref="A2:J65531"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="130" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -636,7 +721,7 @@
     <row r="2" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="5"/>
@@ -645,8 +730,8 @@
     </row>
     <row r="3" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="6" t="s">
-        <v>1</v>
+      <c r="B3" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
@@ -655,8 +740,8 @@
     </row>
     <row r="4" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="4" t="s">
-        <v>0</v>
+      <c r="B4" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="5"/>
@@ -672,183 +757,186 @@
       <c r="F5" s="5"/>
     </row>
     <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="8" t="s">
-        <v>3</v>
-      </c>
+      <c r="B7" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="19"/>
       <c r="F7" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="I7" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="I9" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="C11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="I9" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+      <c r="I11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" s="9" t="s">
+      <c r="C15" s="18"/>
+      <c r="D15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="9" t="s">
+      <c r="G15" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="9" t="s">
+      <c r="C16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="9" t="s">
+      <c r="G16" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="16"/>
+      <c r="C17" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="16"/>
+      <c r="C18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="C19" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="16"/>
+      <c r="C20" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="9"/>
-      <c r="C15" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
+      <c r="D20" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="16"/>
+      <c r="C21" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
-      <c r="C17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
-      <c r="C18" s="9" t="s">
+      <c r="D21" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
-      <c r="C20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="10"/>
-      <c r="C21" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="65531" spans="2:3" x14ac:dyDescent="0.25">
@@ -856,9 +944,10 @@
       <c r="C65531" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B16:B18"/>
     <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B15:C15"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:D5">
     <cfRule type="duplicateValues" dxfId="0" priority="6"/>

</xml_diff>

<commit_message>
Thêm lọc dashboard theo trường
</commit_message>
<xml_diff>
--- a/Services/Server/Server.API/wwwroot/Reports/BAOCAOTONGQUAN.xlsx
+++ b/Services/Server/Server.API/wwwroot/Reports/BAOCAOTONGQUAN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ACS Solutions\Projects\AMMS_DiemDanhHocSinh\Services\Server\Server.API\wwwroot\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C58C91-729E-4499-A1C0-DDC1E5645CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5344AC34-31C4-4EC2-A0BC-D0C07812FEEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,14 +18,14 @@
   <definedNames>
     <definedName name="datas">#REF!</definedName>
     <definedName name="items">DashBoard!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">DashBoard!$A$1:$N$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">DashBoard!$A$1:$N$36</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>BÁO CÁO TỔNG QUAN</t>
   </si>
@@ -200,6 +200,26 @@
   </si>
   <si>
     <t>{{item.TotalSchoolModel.TotalStudent}}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>School:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  {{organizationName}}</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -390,6 +410,11 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -399,11 +424,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,10 +718,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:J65531"/>
+  <dimension ref="A2:J65532"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="130" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -731,7 +751,7 @@
     <row r="3" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
@@ -741,215 +761,225 @@
     <row r="4" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="C4" s="6"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="4"/>
+      <c r="B5" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="20" t="s">
+    <row r="6" spans="1:10" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="19"/>
-      <c r="F7" s="12" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="16"/>
+      <c r="F8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="I7" s="14" t="s">
+      <c r="G8" s="13"/>
+      <c r="I8" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="15"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G8" s="3"/>
+      <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="I9" s="10" t="s">
+      <c r="G10" s="3"/>
+      <c r="I10" s="10" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C13" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I13" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J13" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F15" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="17" t="s">
+    <row r="16" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="8" t="s">
+      <c r="C16" s="21"/>
+      <c r="D16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G16" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F17" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G17" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="16"/>
-      <c r="C17" s="8" t="s">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="19"/>
+      <c r="C18" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D18" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F18" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G18" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="16"/>
-      <c r="C18" s="8" t="s">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="19"/>
+      <c r="C19" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D19" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="16" t="s">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D20" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="16"/>
-      <c r="C20" s="8" t="s">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="19"/>
+      <c r="C21" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D21" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="16"/>
-      <c r="C21" s="8" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="19"/>
+      <c r="C22" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D22" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="65531" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65531" s="2"/>
-      <c r="C65531" s="2"/>
+    <row r="65532" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65532" s="2"/>
+      <c r="C65532" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B16:C16"/>
   </mergeCells>
-  <conditionalFormatting sqref="A2:D5">
+  <conditionalFormatting sqref="A2:D6">
     <cfRule type="duplicateValues" dxfId="0" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>

</xml_diff>